<commit_message>
Rework subcalc calcsand include a Python backup to the C extension, add emf.fields.enviro
</commit_message>
<xml_diff>
--- a/emf/subcalc/subcalc-tower-template.xlsx
+++ b/emf/subcalc/subcalc-tower-template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\EMF_Resources\mmb-python-package\emf\subcalc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -26,9 +31,6 @@
     <t>Integer defining the sequence of towers in the same group, determining the order in which wires are strung between towers</t>
   </si>
   <si>
-    <t>The rotation of the tower in degrees, where 0 is along the positive x axis, increasing toward the positive y axis</t>
-  </si>
-  <si>
     <t>x coordinate of the tower/pole in the model domain (ft)</t>
   </si>
   <si>
@@ -72,13 +74,16 @@
   </si>
   <si>
     <t>phase</t>
+  </si>
+  <si>
+    <t>The rotation of the tower in degrees, where 0 is along the positive x axis, increasing counter-clockwise. The SUBCALC program defines zero rotaion along the negative y axis, which is baffling.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -215,6 +220,14 @@
       <color rgb="FF4D4D4D"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -261,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,9 +306,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,6 +341,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,93 +517,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -606,45 +621,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>